<commit_message>
Revert "renameing 完成 表格更新"
</commit_message>
<xml_diff>
--- a/mod汉化进度.xlsx
+++ b/mod汉化进度.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26221969-8B90-4C89-98E9-DD206AD2E833}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF724803-3D13-4450-812E-FEAF2D811C45}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mod版本与更新日志!$A$6:$D$380</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mod汉化状态!$A$1:$B$188</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">scripts汉化状态!$A$1:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">scripts汉化状态!$A$1:$H$43</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="440">
   <si>
     <t>1.7.10-3.5.1a</t>
   </si>
@@ -1377,29 +1377,6 @@
   </si>
   <si>
     <t>DisplayName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1798,7 +1775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E6D76FF-7B7A-4144-94EA-02F6969C5E2B}">
   <dimension ref="A1:E188"/>
   <sheetViews>
-    <sheetView topLeftCell="A268" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
@@ -5399,7 +5376,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5436,440 +5413,413 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>399</v>
-      </c>
-      <c r="B2" t="s">
-        <v>442</v>
+        <v>396</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>870</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>440</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>402</v>
-      </c>
-      <c r="B3" t="s">
-        <v>442</v>
+        <v>397</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>805</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>440</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>398</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>584</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>440</v>
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>421</v>
+        <v>399</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>435</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>440</v>
+        <v>870</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>422</v>
+        <v>400</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>381</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>440</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>401</v>
       </c>
-      <c r="B7" t="s">
-        <v>442</v>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7">
         <v>326</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>440</v>
+      <c r="G7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>413</v>
-      </c>
-      <c r="B8" t="s">
-        <v>443</v>
+        <v>402</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>189</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>440</v>
+        <v>805</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>423</v>
+        <v>403</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>174</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>440</v>
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>420</v>
+        <v>404</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>168</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>440</v>
+        <v>41</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>406</v>
-      </c>
-      <c r="B11" t="s">
-        <v>442</v>
+        <v>405</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>154</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>440</v>
+        <v>132</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>419</v>
+        <v>406</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>138</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>440</v>
+        <v>154</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>405</v>
-      </c>
-      <c r="B13" t="s">
-        <v>442</v>
+        <v>407</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>132</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>440</v>
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>426</v>
+        <v>408</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>120</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>440</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>416</v>
-      </c>
-      <c r="B15" t="s">
-        <v>443</v>
+        <v>409</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>74</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>440</v>
+        <v>7</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>410</v>
       </c>
-      <c r="B16" t="s">
-        <v>442</v>
+      <c r="B16">
+        <v>1</v>
       </c>
       <c r="C16">
         <v>69</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>440</v>
+      <c r="E16" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>404</v>
-      </c>
-      <c r="B17" t="s">
-        <v>442</v>
+        <v>411</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>41</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>440</v>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>425</v>
-      </c>
-      <c r="B18" t="s">
-        <v>445</v>
+        <v>412</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>41</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>440</v>
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>407</v>
-      </c>
-      <c r="B19" t="s">
-        <v>442</v>
+        <v>413</v>
       </c>
       <c r="C19">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>440</v>
+        <v>189</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>400</v>
-      </c>
-      <c r="B20" t="s">
-        <v>442</v>
+        <v>414</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>440</v>
+        <v>9</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>417</v>
-      </c>
-      <c r="B21" t="s">
-        <v>442</v>
+        <v>415</v>
       </c>
       <c r="C21">
-        <v>14</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>440</v>
+        <v>10</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>415</v>
-      </c>
-      <c r="B22" t="s">
-        <v>443</v>
+        <v>416</v>
       </c>
       <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>440</v>
+        <v>74</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>414</v>
-      </c>
-      <c r="B23" t="s">
-        <v>442</v>
+        <v>417</v>
       </c>
       <c r="C23">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>440</v>
+        <v>14</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>409</v>
-      </c>
-      <c r="B24" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="C24">
-        <v>7</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>440</v>
+        <v>584</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>397</v>
-      </c>
-      <c r="B25" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>440</v>
+        <v>138</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>424</v>
-      </c>
-      <c r="B26" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>440</v>
+        <v>168</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>412</v>
-      </c>
-      <c r="B27" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>408</v>
-      </c>
-      <c r="B28" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>440</v>
+        <v>381</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>396</v>
-      </c>
-      <c r="B29" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>441</v>
+        <v>174</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>398</v>
-      </c>
-      <c r="B30" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>440</v>
+        <v>6</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>403</v>
-      </c>
-      <c r="B31" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>440</v>
+        <v>41</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>411</v>
-      </c>
-      <c r="B32" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>440</v>
+        <v>120</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G32" xr:uid="{1BFB6A51-E435-4AD5-B5E3-1233AA04C29B}">
-    <sortState ref="A2:G32">
-      <sortCondition descending="1" ref="C2:C32"/>
-      <sortCondition ref="B2:B32" customList="Yes"/>
-    </sortState>
-  </autoFilter>
-  <sortState ref="A2:G32">
-    <sortCondition ref="B2:B32" customList="Yes"/>
-    <sortCondition ref="C2:C32"/>
-  </sortState>
+  <autoFilter ref="A1:H43" xr:uid="{4F126F61-AA49-451A-B5A2-594628A094AE}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>